<commit_message>
falta concluir as formulas em toda a planilha - dificuldades em realizar uma das forumas de solidos totais
</commit_message>
<xml_diff>
--- a/cibapp/Laboratorio.xlsx
+++ b/cibapp/Laboratorio.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
   <si>
     <t>Data de incubação</t>
   </si>
@@ -85,40 +85,13 @@
     <t>01/01/2000</t>
   </si>
   <si>
-    <t>thrhr</t>
-  </si>
-  <si>
-    <t>Laboratório</t>
-  </si>
-  <si>
-    <t>AgroIndústria</t>
-  </si>
-  <si>
-    <t>Codigestão</t>
-  </si>
-  <si>
-    <t>Abatedouro de aves</t>
-  </si>
-  <si>
-    <t>Água residual</t>
-  </si>
-  <si>
-    <t>rtrh</t>
-  </si>
-  <si>
-    <t>rthrhrh</t>
-  </si>
-  <si>
-    <t>3434</t>
-  </si>
-  <si>
-    <t>2342</t>
-  </si>
-  <si>
-    <t>23424</t>
-  </si>
-  <si>
-    <t/>
+    <t>IN-18/03/19</t>
+  </si>
+  <si>
+    <t>--Selecione--</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -449,7 +422,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC4"/>
+  <dimension ref="A1:AC7"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
@@ -555,52 +528,76 @@
         <v>24</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="I2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
+      </c>
+      <c r="J2" s="1">
+        <v>61</v>
       </c>
       <c r="K2" s="1">
-        <f t="normal" ca="1">MAXIMO(J2:J4)</f>
+        <f t="normal">MAX(J2:J4)</f>
         <v>0</v>
       </c>
       <c r="L2" s="1">
-        <f t="normal" ca="1">SE(A2=0;;(K2-K3)/K3)</f>
+        <f t="normal">(K2-K3)/K3</f>
         <v>0</v>
       </c>
       <c r="M2" s="1">
-        <f t="normal" ca="1">MÉDIA(J2:J4)</f>
-        <v>0</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>34</v>
+        <f t="normal">AVERAGE(J2:J4)</f>
+        <v>0</v>
+      </c>
+      <c r="N2" s="1">
+        <v>288</v>
+      </c>
+      <c r="O2" s="1">
+        <f t="normal">MAX(N2:N4)</f>
+        <v>0</v>
+      </c>
+      <c r="P2" s="1">
+        <f t="normal">(O2-O3)/O3</f>
+        <v>0</v>
+      </c>
+      <c r="Q2" s="1">
+        <f t="normal">AVERAGE(N2:N4)</f>
+        <v>0</v>
+      </c>
+      <c r="R2" s="1">
+        <f t="normal">(Q2/M2)</f>
+        <v>0</v>
+      </c>
+      <c r="S2" s="1">
+        <v>95</v>
+      </c>
+      <c r="T2" s="1">
+        <f t="normal">AVERAGE(S2:S4)*10</f>
+        <v>0</v>
+      </c>
+      <c r="U2" s="1">
+        <f t="normal">((MAX(S2:S4;1))-(MIN(S2:S4;1)))/(((MAX(S2:S4;1))+(MIN(S2:S4;1)))/2)*100</f>
+        <v>0</v>
+      </c>
+      <c r="V2" s="1">
+        <v>64</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>664</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:29" s="1" customFormat="1" customHeight="0">
@@ -613,27 +610,31 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="1" t="s">
-        <v>32</v>
+      <c r="J3" s="1">
+        <v>56</v>
       </c>
       <c r="K3" s="1">
-        <f t="normal" ca="1">MÍNIMO(J2:J4)</f>
-        <v>0</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AB3" s="1" t="s">
-        <v>34</v>
+        <f t="normal">MIN(J2:J4)</f>
+        <v>0</v>
+      </c>
+      <c r="N3" s="1">
+        <v>302</v>
+      </c>
+      <c r="O3" s="1">
+        <f t="normal">MIN(N2:N4)</f>
+        <v>0</v>
+      </c>
+      <c r="S3" s="1">
+        <v>897</v>
+      </c>
+      <c r="V3" s="1">
+        <v>897</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>456</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:29" s="1" customFormat="1" customHeight="0">
@@ -646,27 +647,176 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AB4" s="1" t="s">
-        <v>34</v>
+      <c r="J4" s="1">
+        <v>59</v>
+      </c>
+      <c r="N4" s="1">
+        <v>321</v>
+      </c>
+      <c r="S4" s="1">
+        <v>95</v>
+      </c>
+      <c r="V4" s="1">
+        <v>64</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>986</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" s="1" customFormat="1" customHeight="0">
+      <c r="A5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="1">
+        <v>61</v>
+      </c>
+      <c r="K5" s="1">
+        <f t="normal" ca="1">MAX(J5:J7)</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
+        <f t="normal" ca="1">(K5-K6)/K6</f>
+        <v>0</v>
+      </c>
+      <c r="M5" s="1">
+        <f t="normal" ca="1">AVERAGE(J5:J7)</f>
+        <v>0</v>
+      </c>
+      <c r="N5" s="1">
+        <v>288</v>
+      </c>
+      <c r="O5" s="1">
+        <f t="normal" ca="1">MAX(N5:N7)</f>
+        <v>0</v>
+      </c>
+      <c r="P5" s="1">
+        <f t="normal" ca="1">(O5-O6)/O6</f>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="1">
+        <f t="normal" ca="1">AVERAGE(N5:N7)</f>
+        <v>0</v>
+      </c>
+      <c r="R5" s="1">
+        <f t="normal" ca="1">(Q5/M5)</f>
+        <v>0</v>
+      </c>
+      <c r="S5" s="1">
+        <v>95</v>
+      </c>
+      <c r="T5" s="1">
+        <f t="normal" ca="1">AVERAGE(S5:S7)*10</f>
+        <v>0</v>
+      </c>
+      <c r="U5" s="1">
+        <f t="normal" ca="1">((MAX(S5:S7;1))-(MIN(S5:S7;1)))/(((MAX(S5:S7;1))+(MIN(S5:S7;1)))/2)*100</f>
+        <v>0</v>
+      </c>
+      <c r="V5" s="1">
+        <v>64</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>664</v>
+      </c>
+      <c r="AB5" s="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" s="1" customFormat="1" customHeight="0">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1">
+        <v>56</v>
+      </c>
+      <c r="K6" s="1">
+        <f t="normal" ca="1">MIN(J5:J7)</f>
+        <v>0</v>
+      </c>
+      <c r="N6" s="1">
+        <v>302</v>
+      </c>
+      <c r="O6" s="1">
+        <f t="normal" ca="1">MIN(N5:N7)</f>
+        <v>0</v>
+      </c>
+      <c r="S6" s="1">
+        <v>79</v>
+      </c>
+      <c r="V6" s="1">
+        <v>64</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>456</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" s="1" customFormat="1" customHeight="0">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1">
+        <v>59</v>
+      </c>
+      <c r="N7" s="1">
+        <v>321</v>
+      </c>
+      <c r="S7" s="1">
+        <v>95</v>
+      </c>
+      <c r="V7" s="1">
+        <v>64</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>986</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="18">
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:C4"/>
@@ -676,6 +826,15 @@
     <mergeCell ref="G2:G4"/>
     <mergeCell ref="H2:H4"/>
     <mergeCell ref="I2:I4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="G5:G7"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="I5:I7"/>
   </mergeCells>
   <pageSetup/>
 </worksheet>

</xml_diff>